<commit_message>
simplify genereic ac battety model
set absolute standby losses to zero W
</commit_message>
<xml_diff>
--- a/input/PerModPAR.xlsx
+++ b/input/PerModPAR.xlsx
@@ -1425,9 +1425,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>330840</xdr:colOff>
+      <xdr:colOff>330480</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>137520</xdr:rowOff>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1441,7 +1441,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4947480" y="261000"/>
-          <a:ext cx="9282600" cy="3305520"/>
+          <a:ext cx="9282240" cy="3305160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1467,9 +1467,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1479,7 +1479,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11886840" cy="7837560"/>
+          <a:ext cx="11887200" cy="7837200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1512,9 +1512,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1524,7 +1524,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11886840" cy="7837560"/>
+          <a:ext cx="11887200" cy="7837200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1557,9 +1557,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1569,7 +1569,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11886840" cy="7837560"/>
+          <a:ext cx="11887200" cy="7837200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1602,9 +1602,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1614,7 +1614,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11886840" cy="7837560"/>
+          <a:ext cx="11887200" cy="7837200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1647,9 +1647,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1659,7 +1659,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11886840" cy="7837560"/>
+          <a:ext cx="11887200" cy="7837200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1692,9 +1692,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1704,7 +1704,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11886840" cy="7837560"/>
+          <a:ext cx="11887200" cy="7837200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1737,9 +1737,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1749,7 +1749,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11886840" cy="7837560"/>
+          <a:ext cx="11887200" cy="7837200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1782,9 +1782,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1794,7 +1794,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11886840" cy="7837560"/>
+          <a:ext cx="11887200" cy="7837200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1827,9 +1827,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1839,7 +1839,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11886840" cy="7837560"/>
+          <a:ext cx="11887200" cy="7837200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1872,9 +1872,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1884,7 +1884,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11886840" cy="7837560"/>
+          <a:ext cx="11887200" cy="7837200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1917,9 +1917,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1929,7 +1929,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11886840" cy="7837560"/>
+          <a:ext cx="11887200" cy="7837200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1962,9 +1962,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1974,7 +1974,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11886840" cy="7837560"/>
+          <a:ext cx="11887200" cy="7837200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2007,9 +2007,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2019,7 +2019,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11886840" cy="7837560"/>
+          <a:ext cx="11887200" cy="7837200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2052,9 +2052,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2064,7 +2064,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11886840" cy="7837560"/>
+          <a:ext cx="11887200" cy="7837200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2097,9 +2097,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2109,7 +2109,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11886840" cy="7837560"/>
+          <a:ext cx="11887200" cy="7837200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2142,9 +2142,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2154,7 +2154,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11886840" cy="7837560"/>
+          <a:ext cx="11887200" cy="7837200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2187,9 +2187,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2199,7 +2199,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11886840" cy="7837560"/>
+          <a:ext cx="11887200" cy="7837200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2232,9 +2232,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2244,7 +2244,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11886840" cy="7837560"/>
+          <a:ext cx="11887200" cy="7837200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2277,9 +2277,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2289,7 +2289,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11886840" cy="7837560"/>
+          <a:ext cx="11887200" cy="7837200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2322,9 +2322,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2334,7 +2334,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11886840" cy="7837560"/>
+          <a:ext cx="11887200" cy="7837200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2367,9 +2367,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2379,7 +2379,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11886840" cy="7837560"/>
+          <a:ext cx="11887200" cy="7837200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2412,9 +2412,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2424,7 +2424,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11886840" cy="7837560"/>
+          <a:ext cx="11887200" cy="7837200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2457,9 +2457,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2469,7 +2469,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11886840" cy="7837560"/>
+          <a:ext cx="11887200" cy="7837200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2502,9 +2502,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2514,7 +2514,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11886840" cy="7837560"/>
+          <a:ext cx="11887200" cy="7837200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2547,9 +2547,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2559,7 +2559,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11886840" cy="7837560"/>
+          <a:ext cx="11887200" cy="7837200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2592,9 +2592,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2604,7 +2604,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11886840" cy="7837560"/>
+          <a:ext cx="11887200" cy="7837200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2637,9 +2637,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2649,7 +2649,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11886840" cy="7837560"/>
+          <a:ext cx="11887200" cy="7837200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2682,9 +2682,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2694,7 +2694,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11886840" cy="7837560"/>
+          <a:ext cx="11887200" cy="7837200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2727,9 +2727,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2739,7 +2739,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11886840" cy="7837560"/>
+          <a:ext cx="11887200" cy="7837200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2772,9 +2772,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2784,7 +2784,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11886840" cy="7837560"/>
+          <a:ext cx="11887200" cy="7837200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2817,9 +2817,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2829,7 +2829,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11886840" cy="7837560"/>
+          <a:ext cx="11887200" cy="7837200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2862,9 +2862,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2874,7 +2874,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11886840" cy="7837560"/>
+          <a:ext cx="11887200" cy="7837200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2907,9 +2907,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135720</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2919,7 +2919,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11886840" cy="7837560"/>
+          <a:ext cx="11887200" cy="7837200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3134,7 +3134,7 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -3152,14 +3152,14 @@
   <dimension ref="A1:AMJ228"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="7" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="7" topLeftCell="G113" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="A113" activeCellId="0" sqref="A113"/>
+      <selection pane="bottomRight" activeCell="G61" activeCellId="0" sqref="G61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="15.49"/>
@@ -3171,7 +3171,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="16.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="6" width="18.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="5" width="19.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="4" width="16.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="4" width="16.14"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="14" style="7" width="8.83"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="15" style="5" width="8.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
@@ -5289,7 +5289,7 @@
         <v>92</v>
       </c>
       <c r="G53" s="5" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H53" s="5" t="n">
         <v>14.9</v>
@@ -5338,7 +5338,7 @@
         <v>92</v>
       </c>
       <c r="G54" s="5" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="H54" s="5" t="n">
         <v>0.1</v>
@@ -5418,7 +5418,7 @@
         <v>92</v>
       </c>
       <c r="G56" s="5" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H56" s="5" t="n">
         <v>12.1</v>
@@ -5598,7 +5598,7 @@
         <v>92</v>
       </c>
       <c r="G60" s="23" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H60" s="5" t="n">
         <v>1</v>
@@ -10207,7 +10207,7 @@
     <mergeCell ref="O1:R1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>